<commit_message>
tugas 1,2,3 menu user
</commit_message>
<xml_diff>
--- a/public/template_kategori.xlsx
+++ b/public/template_kategori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540B1C5B-49E7-43AF-AFA5-A248BEA3FF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9DC7AA-A9E7-437D-A563-B47018F496F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10872" yWindow="708" windowWidth="12108" windowHeight="8964" xr2:uid="{19C5E304-C9FA-4C50-9B98-331AADE9E6B7}"/>
+    <workbookView xWindow="192" yWindow="1128" windowWidth="12108" windowHeight="8964" xr2:uid="{19C5E304-C9FA-4C50-9B98-331AADE9E6B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>kategori_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>kategori_kode</t>
   </si>
@@ -475,85 +472,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AFAEB8-1175-4E15-A867-61486E4C4572}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>